<commit_message>
Includes all current IETF issues from the issue tracker.
</commit_message>
<xml_diff>
--- a/AODVv2-issues.xlsx
+++ b/AODVv2-issues.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="151">
   <si>
     <t xml:space="preserve">Ticket </t>
   </si>
@@ -435,6 +435,39 @@
   </si>
   <si>
     <t>Need to further restrict "LoopFree" condition</t>
+  </si>
+  <si>
+    <t>#58</t>
+  </si>
+  <si>
+    <t>Definitions of OrigNode and TargNode (Submitted for Justin Dean)</t>
+  </si>
+  <si>
+    <t>#59</t>
+  </si>
+  <si>
+    <t>Use of the term "invalid" (Submitted for Justin Dean)</t>
+  </si>
+  <si>
+    <t>Charles Perkins</t>
+  </si>
+  <si>
+    <t>#60</t>
+  </si>
+  <si>
+    <t>Should OrigNode be included in the message header? (Submitted for Justin Dean)</t>
+  </si>
+  <si>
+    <t>#61</t>
+  </si>
+  <si>
+    <t>Difference between "broken" and "expired" (Submitted for Justin Dean)</t>
+  </si>
+  <si>
+    <t>#62</t>
+  </si>
+  <si>
+    <t>Inconsistency surrounding the "timed" state (Submitted for Justin Dean)</t>
   </si>
 </sst>
 </file>
@@ -786,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" activeCellId="1" sqref="A15:XFD15 A15:XFD15"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,6 +2179,121 @@
         <v>41913</v>
       </c>
     </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" t="s">
+        <v>59</v>
+      </c>
+      <c r="F59" t="s">
+        <v>17</v>
+      </c>
+      <c r="G59" t="s">
+        <v>137</v>
+      </c>
+      <c r="H59" t="s">
+        <v>14</v>
+      </c>
+      <c r="I59" s="1">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>142</v>
+      </c>
+      <c r="B60" t="s">
+        <v>143</v>
+      </c>
+      <c r="C60" t="s">
+        <v>59</v>
+      </c>
+      <c r="F60" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" t="s">
+        <v>144</v>
+      </c>
+      <c r="H60" t="s">
+        <v>14</v>
+      </c>
+      <c r="I60" s="1">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>145</v>
+      </c>
+      <c r="B61" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" t="s">
+        <v>59</v>
+      </c>
+      <c r="F61" t="s">
+        <v>24</v>
+      </c>
+      <c r="G61" t="s">
+        <v>144</v>
+      </c>
+      <c r="H61" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" s="1">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>147</v>
+      </c>
+      <c r="B62" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" t="s">
+        <v>59</v>
+      </c>
+      <c r="F62" t="s">
+        <v>24</v>
+      </c>
+      <c r="G62" t="s">
+        <v>144</v>
+      </c>
+      <c r="H62" t="s">
+        <v>14</v>
+      </c>
+      <c r="I62" s="1">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>149</v>
+      </c>
+      <c r="B63" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" t="s">
+        <v>59</v>
+      </c>
+      <c r="F63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G63" t="s">
+        <v>144</v>
+      </c>
+      <c r="H63" t="s">
+        <v>14</v>
+      </c>
+      <c r="I63" s="1">
+        <v>41991</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2153,10 +2301,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,6 +3486,121 @@
         <v>41913</v>
       </c>
     </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>58</v>
+      </c>
+      <c r="B52" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" t="s">
+        <v>137</v>
+      </c>
+      <c r="F52" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" s="1">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>59</v>
+      </c>
+      <c r="B53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" t="s">
+        <v>144</v>
+      </c>
+      <c r="F53" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" s="1">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>60</v>
+      </c>
+      <c r="B54" t="s">
+        <v>146</v>
+      </c>
+      <c r="C54" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" t="s">
+        <v>144</v>
+      </c>
+      <c r="F54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" s="1">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>61</v>
+      </c>
+      <c r="B55" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" t="s">
+        <v>144</v>
+      </c>
+      <c r="F55" t="s">
+        <v>14</v>
+      </c>
+      <c r="G55" s="1">
+        <v>41991</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>62</v>
+      </c>
+      <c r="B56" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" t="s">
+        <v>144</v>
+      </c>
+      <c r="F56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="1">
+        <v>41991</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:G51">
     <sortCondition ref="A2:A51"/>

</xml_diff>